<commit_message>
started the linking table
</commit_message>
<xml_diff>
--- a/Docs/gantt-chart.xlsx
+++ b/Docs/gantt-chart.xlsx
@@ -5,7 +5,7 @@
   <workbookPr filterPrivacy="1"/>
   <xr:revisionPtr revIDLastSave="41" documentId="8_{F6A95013-7850-4FD5-A972-A79D16D08BE0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CB43A600-3FE0-4968-A7B6-BA7BD1793182}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
+    <workbookView xWindow="4230" yWindow="3195" windowWidth="28755" windowHeight="15285" xr2:uid="{83E43DC8-C7A0-4A4D-AAF4-DA46DABAE971}"/>
   </bookViews>
   <sheets>
     <sheet name="Project Tracker" sheetId="4" r:id="rId1"/>
@@ -1270,7 +1270,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{874596C9-4480-42E1-AED8-9CD36477B807}" type="CELLRANGE">
+                    <a:fld id="{EA678B93-E222-4409-8E8A-A20C844E62D7}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1303,7 +1303,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{E63E84E6-31C2-4FF0-B80D-1FE2EE041FA5}" type="CELLRANGE">
+                    <a:fld id="{3807BA3D-5816-4BBA-AC64-CB63E31B7747}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1336,7 +1336,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C5882696-6314-453A-9C38-CCD9FCF9A261}" type="CELLRANGE">
+                    <a:fld id="{31436C6E-2084-4A5C-8A83-6830ED56D4FE}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1369,7 +1369,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{BF0A6C6A-CD4E-4156-8BDF-7389A449659F}" type="CELLRANGE">
+                    <a:fld id="{0F129C8D-F3CB-44AD-B9D5-33D71C678358}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1402,7 +1402,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{C031AFD5-F6DF-483C-B5DF-1B60FD2FFE62}" type="CELLRANGE">
+                    <a:fld id="{896D86ED-901F-4E56-9EDC-C24365E393E8}" type="CELLRANGE">
                       <a:rPr lang="en-IE"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3357,26 +3357,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Url xsi:nil="true"/>
-      <Description xsi:nil="true"/>
-    </Image>
-    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
-    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </ImageTagsTaxHTField>
-    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
-    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010079F111ED35F8CC479449609E8A0923A6" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2d714a3296df14eba7a100bb665443ca">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xmlns:ns3="16c05727-aa75-4e4a-9b5f-8a80a1165891" xmlns:ns4="230e9df3-be65-4c73-a93b-d1236ebd677e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="49549bf45bfbbfb6cffed527380e77e1" ns1:_="" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3664,6 +3644,26 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <Image xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Url xsi:nil="true"/>
+      <Description xsi:nil="true"/>
+    </Image>
+    <Status xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">Not started</Status>
+    <Background xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">false</Background>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <ImageTagsTaxHTField xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </ImageTagsTaxHTField>
+    <TaxCatchAll xmlns="230e9df3-be65-4c73-a93b-d1236ebd677e" xsi:nil="true"/>
+    <MediaServiceKeyPoints xmlns="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -3674,18 +3674,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E831BF2-0015-415C-9D2C-7A347CF05F14}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
-    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7571AF33-E002-4236-8CE7-43F9F2A643B8}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3706,6 +3694,25 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7E831BF2-0015-415C-9D2C-7A347CF05F14}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="16c05727-aa75-4e4a-9b5f-8a80a1165891"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="230e9df3-be65-4c73-a93b-d1236ebd677e"/>
+    <ds:schemaRef ds:uri="71af3243-3dd4-4a8d-8c0d-dd76da1f02a5"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F876E90C-8EDE-4D57-B08F-186FE12CD4D8}">
   <ds:schemaRefs>

</xml_diff>